<commit_message>
fixed seed, added outputs/fft-o__Bacteroidales_pruned.xlsx
</commit_message>
<xml_diff>
--- a/outputs/fft-o__Bacteroidales_pruned.xlsx
+++ b/outputs/fft-o__Bacteroidales_pruned.xlsx
@@ -31,6 +31,10 @@
     <sheet name="g__C941_wrapper-SH20" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="g__C941_wrapper-SH21" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="g__C941_wrapper-SH-c" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="g__C941_wrapper-SH22" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="g__C941_wrapper-SH-c1" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="g__C941_wrapper-SH23" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="g__C941_wrapper-SH-c2" sheetId="29" state="visible" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -8277,13 +8281,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -8304,7 +8308,7 @@
         <v>0.7601939990927784</v>
       </c>
       <c r="D3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -8319,13 +8323,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -8346,7 +8350,7 @@
         <v>0.5027908787874961</v>
       </c>
       <c r="D5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -8361,13 +8365,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -8382,13 +8386,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -8403,13 +8407,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -8424,13 +8428,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
         <v>0.9156284002549644</v>
       </c>
       <c r="D9" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -8445,13 +8449,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -8466,13 +8470,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -8487,13 +8491,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -8508,13 +8512,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -8529,13 +8533,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -8550,13 +8554,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -8577,7 +8581,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -8592,13 +8596,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -8613,13 +8617,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -8634,13 +8638,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -8655,13 +8659,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -8676,13 +8680,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0.09068564601933804</v>
       </c>
       <c r="D21" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -8697,13 +8701,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -8718,13 +8722,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -8739,13 +8743,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -8760,13 +8764,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -8781,13 +8785,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0.5280149502448542</v>
       </c>
       <c r="D26" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -8808,7 +8812,7 @@
         <v>0.7282496126011326</v>
       </c>
       <c r="D27" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -8823,13 +8827,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -8844,13 +8848,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -8865,13 +8869,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -8886,13 +8890,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -8907,10 +8911,3114 @@
         </is>
       </c>
       <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>RUG506</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>RUG434</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>RUG228</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>RUG496</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>f__UBA932</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>prediction</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>RUG401</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-11.77064991365607</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.569031643323741</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-3.893772334583864</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>RUG354</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.6981184875712405</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.888030033869266</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-7.450751823280592</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>RUG462</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-10.54233447642197</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3.534740603446946</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-4.165413443785486</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>RUG362</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8.923883093226515</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1.379645501912714</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-6.857663462320843</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>RUG494</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-12.74263956629608</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.471740757664703</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-4.949308618804961</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>RUG559</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-9.731531521318022</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6.426933830776401</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-6.8387672060956</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>RUG575</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-7.207624215272088</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.297876378522352</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-7.209907947068752</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>RUG396</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-10.57541682844611</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2.29754503453491</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-3.564181135600138</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>RUG378</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-2.43238873000256</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4.288927217110628</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-7.025062529090888</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>RUG558</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-14.24492453221204</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.732240087334143</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-4.1117575498468</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>RUG549</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-8.781571274675882</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.500917278657682</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-4.590613099543096</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>RUG548</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-15.04033211796783</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.246340827362927</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-1.666997072919273</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>hRUG888</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-15.89276420926017</v>
+      </c>
+      <c r="C14" t="n">
+        <v>9.940224829915183</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-7.294968584809325</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>RUG278</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-12.72316893806738</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2.44065982473505</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-3.319380302676965</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>RUG755</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-2.172356679488189</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.054780932029603</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-4.272499935692285</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>RUG723</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>-11.88192696854524</v>
+      </c>
+      <c r="C17" t="n">
+        <v>5.977539973938859</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-6.051536867621008</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>RUG497</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-13.27558264004629</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2.61386923882444</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-3.24117481640684</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>RUG490</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-12.05401875500686</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.696585632029629</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-7.076619143946857</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>RUG379</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-11.67282928657851</v>
+      </c>
+      <c r="C20" t="n">
+        <v>6.444815263507425</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-6.187335148483489</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>RUG412</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.4151571320491887</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-1.988807400323672</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-3.593592395472844</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>RUG507</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-17.90941225621241</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3.281596980352975</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-2.982551975408762</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>RUG485</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-9.100779508466704</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.271587358544016</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-2.533699816277757</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>RUG482</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-6.798290012401067</v>
+      </c>
+      <c r="C24" t="n">
+        <v>6.922606359027858</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-7.425081152297892</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>RUG639</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-3.177495494255861</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1.636490052138625</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-4.19665287836915</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>RUG519</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.9142228836658645</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2.191082776766987</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-7.666194422450939</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>RUG800</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>4.087570431236478</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.897992354476259</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-6.448657362147974</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>RUG330</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>-7.244108083549428</v>
+      </c>
+      <c r="C28" t="n">
+        <v>3.543479165730305</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-4.772888330221288</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>RUG269</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-15.41136268641034</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2.770560757686864</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-3.243648846815926</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>hRUG857</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>-17.34312253450156</v>
+      </c>
+      <c r="C30" t="n">
+        <v>8.185064363768142</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-4.737808204809862</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>RUG532</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-6.258879984153328</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1.116377263532718</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-5.558969919938615</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>RUG373</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-9.09921124455609</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.4560669134072931</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-2.892939871369625</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>RUG506</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-11.39174421491136</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1.860660378261961</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-3.487468605161848</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>RUG434</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-18.67853956793012</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8.308646776591639</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-5.021449978020373</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>RUG228</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-2.98372942191705</v>
+      </c>
+      <c r="C35" t="n">
+        <v>4.145712281325252</v>
+      </c>
+      <c r="D35" t="n">
+        <v>-7.452478126683381</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>RUG496</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.7118075135824543</v>
+      </c>
+      <c r="C36" t="n">
+        <v>4.483894717329359</v>
+      </c>
+      <c r="D36" t="n">
+        <v>-8.329333000330614</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>f__UBA932</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>prediction</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>RUG401</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>RUG354</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.8490592437856203</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>RUG462</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>RUG362</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>RUG494</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>RUG559</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>RUG575</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>RUG396</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>RUG378</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>RUG558</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>RUG549</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>RUG548</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>hRUG888</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>RUG278</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>RUG755</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>RUG723</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>RUG497</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>RUG490</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>RUG379</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>RUG412</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.2924214339754057</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>RUG507</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>RUG485</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>RUG482</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>RUG639</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>RUG519</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.9571114418329323</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>RUG800</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.9489961772381295</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>RUG330</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>RUG269</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>hRUG857</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>RUG532</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>RUG373</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.7280334567036466</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>RUG506</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>RUG434</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>RUG228</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>RUG496</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.1440962432087728</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>f__UBA932</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>prediction</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>RUG401</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-3.293243108447888</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.004481283538212</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-4.875766790667459</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>RUG354</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-1.881683260752303</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.130287145216437</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-8.121407535194823</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>RUG462</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-4.704178564349314</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4.300062060101656</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5.592528689482421</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>RUG362</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2.732127760881656</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5156284441414208</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-7.326410242907405</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>RUG494</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-3.725640808931273</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.120523578431744</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-4.720113731149233</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>RUG559</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-6.833265937666641</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4.671446753727736</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-7.163320184882449</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>RUG575</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-5.135392318943737</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.998710346227574</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-7.304880156765497</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>RUG396</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-5.01197400442733</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.6072984276320239</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-3.285790376060666</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>RUG378</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-3.355018745133942</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.789543640685556</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-6.578937007727868</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>RUG558</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-8.249739232879042</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.234905466320292</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-3.268437657170067</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>RUG549</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-3.796516883172661</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4.289322925149514</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-6.194168079823592</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>RUG548</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-4.063781687844656</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3.331767890063725</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-1.56350294736097</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>hRUG888</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-11.17812891276079</v>
+      </c>
+      <c r="C14" t="n">
+        <v>6.277929327463113</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-9.035720846905319</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>RUG278</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-4.530890496900144</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1.378341468805424</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-4.627326980355025</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>RUG755</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-1.634835307237521</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2.337508475090832</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-5.535298243808557</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>RUG723</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>-1.569635203475062</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2.372013190706719</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-6.726689540014752</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>RUG497</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-4.607684720431985</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.794448715383068</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-3.246905845169533</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>RUG490</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-5.72725787834306</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.402549933003756</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-6.136953739598323</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>RUG379</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-6.803809909984963</v>
+      </c>
+      <c r="C20" t="n">
+        <v>8.528809807490761</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-6.275349141575256</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>RUG412</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-1.883421102138761</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-1.308329857292017</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-3.906606046114351</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>RUG507</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-9.294538461586587</v>
+      </c>
+      <c r="C22" t="n">
+        <v>5.323905538219208</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-3.319121257419981</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>RUG485</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-5.407426888091988</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2.383560551342449</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-2.804542183684856</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>RUG482</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-2.283589836575696</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4.636473773085794</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-8.921980963479479</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>RUG639</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-1.927035751334389</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2.21377820369433</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-4.551102340008553</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>RUG519</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-2.581055260614055</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.7876713991209146</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-8.052895911193787</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>RUG800</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.245023826230533</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2.256339452777845</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-6.45932747843591</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>RUG330</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>-4.738431587819741</v>
+      </c>
+      <c r="C28" t="n">
+        <v>3.853478183692228</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-5.236629619497299</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>RUG269</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-6.808033408441987</v>
+      </c>
+      <c r="C29" t="n">
+        <v>4.089537569270255</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-3.671884699581957</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>hRUG857</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>-8.296643330481881</v>
+      </c>
+      <c r="C30" t="n">
+        <v>4.797263604550609</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-5.658864527053866</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>RUG532</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-5.239628756720805</v>
+      </c>
+      <c r="C31" t="n">
+        <v>2.622886452169661</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-4.925660118906763</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>RUG373</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-3.013255379829397</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-0.7623536839720911</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-3.582459111533128</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>RUG506</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-4.628722829600318</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2.922500150447304</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-4.593793709281924</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>RUG434</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-7.465492178096051</v>
+      </c>
+      <c r="C34" t="n">
+        <v>3.5762909304982</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-6.934995904506268</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>RUG228</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-4.998108795822382</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2.506800518056489</v>
+      </c>
+      <c r="D35" t="n">
+        <v>-6.418579010923289</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>RUG496</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.3753969047620266</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2.721202198012663</v>
+      </c>
+      <c r="D36" t="n">
+        <v>-7.79033246162151</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>f__UBA932</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>prediction</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>RUG401</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>-0</v>
       </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>RUG354</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>RUG462</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>RUG362</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7578142220707105</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>f__Bacteroidaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>RUG494</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>RUG559</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>RUG575</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>RUG396</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.803649213816012</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>RUG378</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>RUG558</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>RUG549</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>RUG548</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>hRUG888</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>RUG278</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>RUG755</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>RUG723</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>RUG497</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>RUG490</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>RUG379</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>RUG412</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>RUG507</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>RUG485</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>RUG482</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>RUG639</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>RUG519</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.8938356995604573</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>RUG800</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>RUG330</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>RUG269</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>hRUG857</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>RUG532</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>f__Muribaculaceae</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>RUG373</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-0</v>
+      </c>
       <c r="C32" t="n">
-        <v>-0</v>
+        <v>0.1188231580139544</v>
       </c>
       <c r="D32" t="n">
         <v>-0</v>
@@ -8991,7 +12099,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-0</v>
+        <v>0.3123015476189867</v>
       </c>
       <c r="C36" t="n">
         <v>1</v>

</xml_diff>